<commit_message>
Remove unused language files and add PyInstaller setup instructions
</commit_message>
<xml_diff>
--- a/dist/backup_replacement_data.xlsx
+++ b/dist/backup_replacement_data.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,68 +437,113 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ab</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Anh bảy</t>
-        </is>
-      </c>
+          <t>BEFORE_REPLACEMENT</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>AFTER_REPLACEMENT</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>LINK_EDIT_FILE</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>https://docs.google.com/spreadsheets/d/16uVFfVMKR7jVXA70g4BCo8KAE7iZVYnJT48oTpD1Z-4/edit?gid=0#gid=00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ab</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Anh bảy</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>ac</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>Anh chị
 Hành trình dài quá xa xôi.</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
+    <row r="7">
+      <c r="A7" t="inlineStr">
         <is>
           <t>ddal</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>- Uống thuốc theo toa. Tái khám theo hẹn hoặc khi có dấu hiệu bất thường.
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">- Uống thuốc theo toa. Tái khám theo hẹn hoặc khi có dấu hiệu bất thường.
 - Ăn lạt, nhiều rau xanh, ngũ cốc nguyên hạt…
-- Hạn chế ăn thịt đỏ, nội tạng động vật, mỡ, trứng,tinh bột</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+- Hạn chế ăn thịt đỏ, nội tạng động vật, mỡ, trứng,tinh bột
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
         <is>
           <t>tvptls</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>- Phương pháp phẫu thuật: Laser nội tĩnh mạch hiển hai chân
 - Tư vấn phương pháp phẫu thuật, thời gian, chi phí và các tai biến, biến chứng có thể xảy ra: viêm bầm phỏng da, huyết khối tĩnh mạch,...</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+    <row r="9">
+      <c r="A9" t="inlineStr">
         <is>
           <t>tvstm</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>- Uống thuốc theo toa, tái khám theo hẹn hoặc khi có triệu chứng bất thường
 - Hạn chế tư thế ngồi quá lâu, đứng lâu, ngồi chéo chân hay mang giày cao gót
 - Mang vớ áp lực tĩnh mạch: mang vào ban ngày
 - Tối ngủ kê cao cẳng chân
 - Tập thể dục</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>testso</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>123312</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add language file download and error handling; update GUI button text for reloading data
</commit_message>
<xml_diff>
--- a/dist/backup_replacement_data.xlsx
+++ b/dist/backup_replacement_data.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -544,6 +544,18 @@
       <c r="B10" t="inlineStr">
         <is>
           <t>123312</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>hungvo</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>123$5</t>
         </is>
       </c>
     </row>

</xml_diff>